<commit_message>
Version con Mixer y Premix
</commit_message>
<xml_diff>
--- a/Archivos para Cargas/mixer2.xlsx
+++ b/Archivos para Cargas/mixer2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\programa con Mauro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgonzalez/.bitnami/stackman/machines/xampp/volumes/root/htdocs/feedlot/Archivos para Cargas/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDDC06-5EF9-F546-BDA0-AECA307F74B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">Hoja2!$A$1:$Y$50</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Hoja2!$A$1:$Y$50</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - PESADAS 15-10" description="Conexión a la consulta 'PESADAS 15-10' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - PESADAS 15-10" description="Conexión a la consulta 'PESADAS 15-10' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PESADAS 15-10;Extended Properties=&quot;&quot;" command="SELECT * FROM [PESADAS 15-10]"/>
   </connection>
 </connections>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -283,7 +283,7 @@
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="26">
     <queryTableFields count="25">
       <queryTableField id="1" name="FECHA" tableColumnId="51"/>
@@ -333,34 +333,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PESADAS_15_10" displayName="PESADAS_15_10" ref="A1:Y50" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Y50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PESADAS_15_10" displayName="PESADAS_15_10" ref="A1:Y50" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Y50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="25">
-    <tableColumn id="51" uniqueName="51" name="FECHA" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="52" uniqueName="52" name="HORA" queryTableFieldId="2" dataDxfId="23"/>
-    <tableColumn id="53" uniqueName="53" name="NUM" queryTableFieldId="3" dataDxfId="22"/>
-    <tableColumn id="54" uniqueName="54" name="DESCRIPCION" queryTableFieldId="4" dataDxfId="21"/>
-    <tableColumn id="55" uniqueName="55" name="ING_1" queryTableFieldId="5" dataDxfId="20"/>
-    <tableColumn id="56" uniqueName="56" name="PESO_1" queryTableFieldId="6" dataDxfId="19"/>
-    <tableColumn id="57" uniqueName="57" name="ING_2" queryTableFieldId="7" dataDxfId="18"/>
-    <tableColumn id="58" uniqueName="58" name="PESO_2" queryTableFieldId="8" dataDxfId="17"/>
-    <tableColumn id="59" uniqueName="59" name="ING_3" queryTableFieldId="9" dataDxfId="16"/>
-    <tableColumn id="60" uniqueName="60" name="PESO_3" queryTableFieldId="10" dataDxfId="15"/>
-    <tableColumn id="61" uniqueName="61" name="ING_4" queryTableFieldId="11" dataDxfId="14"/>
-    <tableColumn id="62" uniqueName="62" name="PESO_4" queryTableFieldId="12" dataDxfId="13"/>
-    <tableColumn id="63" uniqueName="63" name="ING_5" queryTableFieldId="13" dataDxfId="12"/>
-    <tableColumn id="64" uniqueName="64" name="PESO_5" queryTableFieldId="14" dataDxfId="11"/>
-    <tableColumn id="65" uniqueName="65" name="ING_6" queryTableFieldId="15" dataDxfId="10"/>
-    <tableColumn id="66" uniqueName="66" name="PESO_6" queryTableFieldId="16" dataDxfId="9"/>
-    <tableColumn id="67" uniqueName="67" name="ING_7" queryTableFieldId="17" dataDxfId="8"/>
-    <tableColumn id="68" uniqueName="68" name="PESO_7" queryTableFieldId="18" dataDxfId="7"/>
-    <tableColumn id="69" uniqueName="69" name="ING_8" queryTableFieldId="19" dataDxfId="6"/>
-    <tableColumn id="70" uniqueName="70" name="PESO_8" queryTableFieldId="20" dataDxfId="5"/>
-    <tableColumn id="71" uniqueName="71" name="ING_9" queryTableFieldId="21" dataDxfId="4"/>
-    <tableColumn id="72" uniqueName="72" name="PESO_9" queryTableFieldId="22" dataDxfId="3"/>
-    <tableColumn id="73" uniqueName="73" name="ING_10" queryTableFieldId="23" dataDxfId="2"/>
-    <tableColumn id="74" uniqueName="74" name="PESO_10" queryTableFieldId="24" dataDxfId="1"/>
-    <tableColumn id="75" uniqueName="75" name="TOTAL" queryTableFieldId="25" dataDxfId="0"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" uniqueName="51" name="FECHA" queryTableFieldId="1" dataDxfId="24"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" uniqueName="52" name="HORA" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" uniqueName="53" name="NUM" queryTableFieldId="3" dataDxfId="22"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" uniqueName="54" name="DESCRIPCION" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" uniqueName="55" name="ING_1" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" uniqueName="56" name="PESO_1" queryTableFieldId="6" dataDxfId="19"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" uniqueName="57" name="ING_2" queryTableFieldId="7" dataDxfId="18"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" uniqueName="58" name="PESO_2" queryTableFieldId="8" dataDxfId="17"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" uniqueName="59" name="ING_3" queryTableFieldId="9" dataDxfId="16"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" uniqueName="60" name="PESO_3" queryTableFieldId="10" dataDxfId="15"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" uniqueName="61" name="ING_4" queryTableFieldId="11" dataDxfId="14"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" uniqueName="62" name="PESO_4" queryTableFieldId="12" dataDxfId="13"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" uniqueName="63" name="ING_5" queryTableFieldId="13" dataDxfId="12"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" uniqueName="64" name="PESO_5" queryTableFieldId="14" dataDxfId="11"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" uniqueName="65" name="ING_6" queryTableFieldId="15" dataDxfId="10"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" uniqueName="66" name="PESO_6" queryTableFieldId="16" dataDxfId="9"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" uniqueName="67" name="ING_7" queryTableFieldId="17" dataDxfId="8"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" uniqueName="68" name="PESO_7" queryTableFieldId="18" dataDxfId="7"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" uniqueName="69" name="ING_8" queryTableFieldId="19" dataDxfId="6"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" uniqueName="70" name="PESO_8" queryTableFieldId="20" dataDxfId="5"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" uniqueName="71" name="ING_9" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" uniqueName="72" name="PESO_9" queryTableFieldId="22" dataDxfId="3"/>
+    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" uniqueName="73" name="ING_10" queryTableFieldId="23" dataDxfId="2"/>
+    <tableColumn id="74" xr3:uid="{00000000-0010-0000-0000-00004A000000}" uniqueName="74" name="PESO_10" queryTableFieldId="24" dataDxfId="1"/>
+    <tableColumn id="75" xr3:uid="{00000000-0010-0000-0000-00004B000000}" uniqueName="75" name="TOTAL" queryTableFieldId="25" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,55 +628,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +741,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43997</v>
       </c>
@@ -830,7 +818,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43997</v>
       </c>
@@ -907,7 +895,7 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43997</v>
       </c>
@@ -984,7 +972,7 @@
         <v>5950</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43997</v>
       </c>
@@ -1061,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43997</v>
       </c>
@@ -1138,7 +1126,7 @@
         <v>6030</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43997</v>
       </c>
@@ -1215,7 +1203,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43997</v>
       </c>
@@ -1292,7 +1280,7 @@
         <v>5840</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44007</v>
       </c>
@@ -1369,7 +1357,7 @@
         <v>5710</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44007</v>
       </c>
@@ -1446,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44007</v>
       </c>
@@ -1523,7 +1511,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44007</v>
       </c>
@@ -1600,7 +1588,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44007</v>
       </c>
@@ -1677,7 +1665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44007</v>
       </c>
@@ -1754,7 +1742,7 @@
         <v>5760</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44007</v>
       </c>
@@ -1831,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44007</v>
       </c>
@@ -1908,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44007</v>
       </c>
@@ -1985,7 +1973,7 @@
         <v>5790</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44007</v>
       </c>
@@ -2062,7 +2050,7 @@
         <v>5670</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44014</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>5710</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44014</v>
       </c>
@@ -2216,7 +2204,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44014</v>
       </c>
@@ -2293,7 +2281,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44014</v>
       </c>
@@ -2370,7 +2358,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44020</v>
       </c>
@@ -2447,7 +2435,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44020</v>
       </c>
@@ -2524,7 +2512,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44020</v>
       </c>
@@ -2601,7 +2589,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44020</v>
       </c>
@@ -2678,7 +2666,7 @@
         <v>5770</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44020</v>
       </c>
@@ -2755,7 +2743,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44020</v>
       </c>
@@ -2832,7 +2820,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44027</v>
       </c>
@@ -2909,7 +2897,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44027</v>
       </c>
@@ -2986,7 +2974,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44027</v>
       </c>
@@ -3063,7 +3051,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44027</v>
       </c>
@@ -3140,7 +3128,7 @@
         <v>5670</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44027</v>
       </c>
@@ -3217,7 +3205,7 @@
         <v>5760</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44027</v>
       </c>
@@ -3294,7 +3282,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44034</v>
       </c>
@@ -3371,7 +3359,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44034</v>
       </c>
@@ -3448,7 +3436,7 @@
         <v>5840</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44034</v>
       </c>
@@ -3525,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44034</v>
       </c>
@@ -3602,7 +3590,7 @@
         <v>5820</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44034</v>
       </c>
@@ -3679,7 +3667,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44034</v>
       </c>
@@ -3756,7 +3744,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44034</v>
       </c>
@@ -3833,7 +3821,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44034</v>
       </c>
@@ -3910,7 +3898,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44041</v>
       </c>
@@ -3987,7 +3975,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44041</v>
       </c>
@@ -4064,7 +4052,7 @@
         <v>5680</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44041</v>
       </c>
@@ -4141,7 +4129,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44041</v>
       </c>
@@ -4218,7 +4206,7 @@
         <v>5690</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44041</v>
       </c>
@@ -4295,7 +4283,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44041</v>
       </c>
@@ -4372,7 +4360,7 @@
         <v>5690</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44103</v>
       </c>
@@ -4449,7 +4437,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44103</v>
       </c>

</xml_diff>